<commit_message>
Orange hrm login page tseting code with data driven
</commit_message>
<xml_diff>
--- a/src/test/resources/Excelsheet/orangehrm.xlsx
+++ b/src/test/resources/Excelsheet/orangehrm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidya\eclipse-workspace\TestingWebsite\src\test\resources\Excelsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidya\eclipse-workspace\Chaintest_testing_project\src\test\resources\Excelsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD28ED3-682F-45C2-99CD-34FE4B8C1E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DEC423-1ADC-4621-9A1A-4F18D9CE9D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{57212ABF-448B-42C4-BE43-B63185AAD6E7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Username</t>
   </si>
@@ -37,13 +37,64 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>dsczdfzs</t>
+  </si>
+  <si>
+    <t>Invalid Username</t>
+  </si>
+  <si>
+    <t>Empty Username</t>
+  </si>
+  <si>
+    <t>EmptyPassword</t>
+  </si>
+  <si>
+    <t>Invalid Password</t>
+  </si>
+  <si>
+    <t>Valid Credentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> this is row 0</t>
+  </si>
+  <si>
+    <t>so on</t>
+  </si>
+  <si>
+    <t>Row Count(for my reference)</t>
+  </si>
+  <si>
+    <t>mmnnn657</t>
+  </si>
+  <si>
+    <t>I wrote code for this</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>this is row 1</t>
+  </si>
+  <si>
+    <t>this is row2</t>
+  </si>
+  <si>
+    <t>this is row3</t>
+  </si>
+  <si>
+    <t>this is row4</t>
+  </si>
+  <si>
+    <t>Inputs(for my reference)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,8 +108,23 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -69,6 +135,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5D3FF"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -99,9 +183,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,41 +513,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84FC32EB-E8C1-4E78-8798-4B61C148A61A}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" customWidth="1"/>
     <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="4" max="4" width="25.21875" customWidth="1"/>
+    <col min="5" max="5" width="29.5546875" customWidth="1"/>
+    <col min="6" max="6" width="41.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1"/>
+      <c r="D2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="C3" s="1"/>
+      <c r="D3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>